<commit_message>
actualización formato propuesta de investigación 15/1172024
</commit_message>
<xml_diff>
--- a/Formato_Propuesta de Investigacion Liga -Desarrollado.xlsx
+++ b/Formato_Propuesta de Investigacion Liga -Desarrollado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Garcia\Desktop\investigación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Garcia\Desktop\METODOLOGIA_INVESTIGACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410E016E-4BCA-42D7-98B5-3894BB5E5955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30C74D1-5013-4AE2-BE8B-7D9B3E027FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Etapa 1. Preparación " sheetId="6" r:id="rId1"/>
@@ -21,16 +21,12 @@
     <sheet name="Etapa 5. Conclusiones" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="108">
   <si>
     <t>Versión: 01</t>
   </si>
@@ -103,12 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve">Técnicas e instrumentos de recolección de información: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conclusiones </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resultados e interpretación </t>
   </si>
   <si>
     <t xml:space="preserve">Registro de búsqueda </t>
@@ -979,13 +969,134 @@
   </si>
   <si>
     <t>Encuesta</t>
+  </si>
+  <si>
+    <t>Se caracteriza por la objetividad y claridad. Se considera la necesidad de que las preguntas sean clara y fáciles de entender evitando el empleo de jerga técnica innecesaria o conceptos amiguios que puedan confundir a los encuestados. Escalas de medición claras( de 1 a 5) para medir la motivación y el rendimiento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS JULIO GARCÍA </t>
+  </si>
+  <si>
+    <t>La encuesta tiene por objetivo recoger información sobre la experiencia de los encuestados en la Liga, con el propósito de diseñar un sistema de gestión que optimice el rendimiento deportivo y a su vez mejore la motivación de los deportistas</t>
+  </si>
+  <si>
+    <t>La participación de los encuestados es muy importante, ya que es una contribución a la mejora de las condiciones en materia de motivación y rendimiento deportivo. La participación del encuestado es voluntaria y sus respuestas son confidenciales. El desarrollo de la encuesta debería tomar entre 10 y 15 minutos para completarse. Tomar el tiempo necesario para responder con sinceridad y reflexionar sobre cada pregunta.</t>
+  </si>
+  <si>
+    <t>DATOS DEMOGRÁFICOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edad:__ Sexo:__ Tiempo practicando el Deporte:___ Categoría:(Infantil, Cadetes, Juvior, U23, Senior). </t>
+  </si>
+  <si>
+    <t>EVALUACIÓN DEL RENDIMIENTO DEPORTIVO:</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5 : Como evaluas tu rendimiento en entrenamientos?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5 : Como evaluas tu rendimiento en competiciones?</t>
+  </si>
+  <si>
+    <t>Falso o Verdadero:         Consideras que el programa de entrenamiento mejora tu rendimiento físico y técnico?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5 : Qué tan satisfecho estás con los entrenadores?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5 : Qué tan satisfecho estás con las instalaciones?</t>
+  </si>
+  <si>
+    <t>MOTIVACIÓN Y  SATISFACCIÓN</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5:  Qué tan motivado te sientes para seguir entrenando?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5:  Qué tan motivado te sientes para seguir compitiendo?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5: Qué tan satisfecho estás con el apoyo emocional y psicológico proporcionado por el equipo y los entrenadores?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5: Sientes que tus expectativas y objetivos están siendo atendidos en la actualidad?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACTORES ASOCIADOS A LA DESERCIÓN </t>
+  </si>
+  <si>
+    <t>Falso o Verdadero: Has considerado alguna vez abandonar la lucha olímpica? Si es Verdadero Por qué?</t>
+  </si>
+  <si>
+    <t>Opción multiple: Cuales son las principales dificultades que enfrentas para seguir participando de tu deporte? 1.- Falta de tiempo 2.-Falta de apoyo financiero 3.- No creo en las capacidades de los entrenadores 4.- No cuento con el apoyo familiar 5.- Otro.</t>
+  </si>
+  <si>
+    <t>PREGUNTA ABIERTA</t>
+  </si>
+  <si>
+    <t>Que elementos te gustaría que se incluyera en un sistema de gestión deportiva en la liga?</t>
+  </si>
+  <si>
+    <t>En una escala de 1 a 5 : Qué tan satisfecho estás con el equipamiento?</t>
+  </si>
+  <si>
+    <t>Falso o Verdadero: Recibes apoyo de tu familia para seguir entrenando y compitiendo?</t>
+  </si>
+  <si>
+    <t>Análisis de los Datos Obtenidos
+Rendimiento en entrenamientos y competiciones:
+Un alto porcentaje de atletas (30% en entrenamientos y 30% en competiciones) se siente satisfecho con su rendimiento (evaluación en 4 o 5). Sin embargo, también hay un porcentaje significativo (25% en entrenamientos y 25% en competiciones) que se encuentra en un nivel neutral. Esto puede sugerir que algunos atletas no están alcanzando sus expectativas personales o las metas del programa de entrenamiento.
+Percepción sobre los entrenadores:
+La satisfacción con los entrenadores es bastante positiva, con un 52.5% de respuestas entre "satisfecho" y "muy satisfecho". Sin embargo, un 17.5% se muestra insatisfecho o neutral, lo que sugiere que puede haber áreas de mejora en la relación entrenador-deportista o en la calidad de los entrenamientos.
+Satisfacción con las instalaciones y equipamiento:
+Las instalaciones y el equipamiento reciben opiniones mixtas. Aproximadamente el 40% de los encuestados están "satisfechos" o "muy satisfechos", pero el 35% restante está neutral o insatisfecho, lo que podría indicar la necesidad de mejorar las condiciones materiales.
+Motivación y apoyo emocional:
+Aunque la mayoría de los atletas se siente motivada tanto para entrenar como para competir (35% motivados o muy motivados), hay un 27.5% que está en una postura neutral o desmotivada, lo que podría indicar una falta de conexión con los objetivos deportivos a nivel personal.
+Apoyo familiar y psicológico:
+El 87.5% de los deportistas afirma recibir apoyo de su familia, lo cual es un factor positivo. Sin embargo, la satisfacción con el apoyo emocional y psicológico proporcionado por los entrenadores es moderada, con un 30% de los atletas expresando insatisfacción o neutralidad.
+Dificultades y razones para la deserción:
+La "falta de apoyo financiero" (30%) y la "falta de tiempo" (25%) son las principales barreras identificadas. Esto refleja un problema común en muchos deportes, donde los atletas enfrentan dificultades económicas o deben balancear el deporte con otros compromisos (como estudios o trabajo).
+La "consideración de abandonar" es una preocupación notable, con un 45% de los encuestados mencionando que han pensado en dejar el deporte, principalmente debido a problemas de salud o falta de tiempo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultados e interpretación 
+Se discriminan los resultados e interpretación de los elementos de información obtenidos de la siguiente forma:              
+Rendimiento en entrenamientos y competiciones:
+Resultado: Un 30% de los atletas están satisfechos con su rendimiento tanto en entrenamientos como en competiciones (calificación de 4 o 5), mientras que un 25% se encuentra neutral (calificación de 3).
+Interpretación: Aunque un número significativo de atletas se siente satisfecho con su rendimiento, un porcentaje considerable se encuentra en un estado neutral. Este dato sugiere que no todos los deportistas están alcanzando sus expectativas o los objetivos establecidos en el programa de entrenamiento. Esto puede indicar la necesidad de ajustes en los métodos de entrenamiento, establecimiento de metas más claras o apoyo adicional para aquellos que no están progresando tan rápido como esperan.
+Percepción sobre los entrenadores:
+Resultado: El 52.5% de los atletas están satisfechos o muy satisfechos con los entrenadores, mientras que el 17.5% está insatisfecho o neutral.
+Interpretación: La percepción sobre los entrenadores es en general positiva, lo que sugiere una relación efectiva en muchos casos. Sin embargo, un porcentaje importante (17.5%) de atletas muestra insatisfacción o indiferencia, lo que puede reflejar áreas de mejora en la comunicación, la calidad de la enseñanza o la adaptación de los entrenamientos a las necesidades individuales de los atletas. Es necesario investigar más a fondo las causas de esta insatisfacción para optimizar la relación entrenador-deportista.
+Satisfacción con las instalaciones y equipamiento:
+Resultado: El 40% de los atletas están satisfechos o muy satisfechos con las instalaciones y el equipamiento, mientras que un 35% está neutral o insatisfecho.
+Interpretación: Las instalaciones y el equipamiento son un aspecto clave en el rendimiento deportivo, y las opiniones mixtas indican que, aunque hay algunos aspectos positivos, un porcentaje considerable de atletas considera que estos factores pueden mejorarse. La falta de satisfacción podría estar relacionada con la insuficiencia o el mal estado del material, lo que puede afectar negativamente la motivación y el rendimiento. Una mejora en este ámbito podría contribuir a un ambiente más adecuado para el entrenamiento y las competiciones.
+Motivación y apoyo emocional:
+Resultado: Un 35% de los atletas se sienten motivados o muy motivados para entrenar y competir, mientras que un 27.5% está neutral o desmotivado.
+Interpretación: La motivación es clave en el rendimiento deportivo, y aunque la mayoría de los atletas está motivada, un 27.5% muestra signos de desmotivación o indiferencia. Esto puede reflejar una desconexión con los objetivos deportivos, una falta de retos adecuados o de apoyo emocional. Es importante identificar las causas específicas de esta desmotivación y trabajar en estrategias de motivación, como el establecimiento de metas personalizadas, reconocimiento y apoyo continuo.
+Apoyo familiar y psicológico:
+Resultado: El 87.5% de los atletas recibe apoyo de su familia, pero la satisfacción con el apoyo emocional y psicológico de los entrenadores es moderada, con un 30% de los atletas expresando insatisfacción o neutralidad.
+Interpretación: El apoyo familiar es un factor clave positivo en la vida de los atletas, lo que probablemente contribuye a su estabilidad y bienestar general. Sin embargo, la satisfacción moderada con el apoyo emocional y psicológico de los entrenadores indica que, aunque algunos entrenadores pueden estar haciendo un buen trabajo, hay espacio para mejorar en cuanto al acompañamiento emocional de los deportistas. Los entrenadores deberían considerar recibir formación adicional en apoyo psicológico y emocional para abordar las necesidades individuales de sus atletas.
+Dificultades y razones para la deserción:
+Resultado: La "falta de apoyo financiero" (30%) y la "falta de tiempo" (25%) son las principales barreras identificadas. Además, el 45% de los atletas han considerado abandonar el deporte, principalmente por problemas de salud o falta de tiempo.
+Interpretación: La falta de apoyo financiero y de tiempo son barreras significativas para la continuidad de los atletas en el deporte. Muchos luchan por equilibrar sus estudios, trabajo y entrenamiento, lo que puede generar estrés y deserción. También, los problemas de salud son una preocupación recurrente. La implementación de un sistema de gestión que ofrezca soluciones a estos problemas (como apoyo financiero o flexibilidad en los horarios de entrenamiento) podría ser crucial para reducir la deserción.
+</t>
+  </si>
+  <si>
+    <t>Conclusiones Conclusiones y Recomendaciones
+Ajustar el programa de entrenamiento: El 25% de los atletas que se encuentran neutrales o insatisfechos con su rendimiento puede indicar que el programa de entrenamiento necesita ser más personalizado o que las expectativas no están alineadas con las capacidades de cada atleta. Se recomienda realizar una evaluación más detallada de las necesidades y metas individuales.
+Mejorar la relación entrenador-deportista: Aunque la mayoría de los atletas están satisfechos con los entrenadores, un 17.5% insatisfecho sugiere que se deben explorar posibles mejoras en la forma de interactuar con los deportistas, así como ofrecer formación en aspectos emocionales y psicológicos del deporte.
+Optimización de las instalaciones y equipamiento: La insatisfacción con las instalaciones y el equipamiento podría abordarse mediante la renovación o ampliación de recursos disponibles para los atletas. Este aspecto tiene un impacto directo sobre la motivación y el rendimiento.
+Estrategias de motivación y apoyo emocional: La desmotivación de un porcentaje de atletas sugiere que se deben implementar estrategias para aumentar la motivación, como el establecimiento de objetivos claros y alcanzables, así como una mayor atención al bienestar emocional de los deportistas.
+Apoyo financiero y gestión de tiempo: Dado que la falta de apoyo financiero y tiempo son las principales barreras para la continuidad, se recomienda buscar alianzas o fuentes de financiamiento que ayuden a aliviar la carga económica de los atletas. Además, flexibilizar los horarios de entrenamiento para acomodar otras responsabilidades podría ayudar a reducir la deserción.
+Atención a la salud física y mental: Dado que el 45% de los atletas ha considerado abandonar debido a problemas de salud, tanto físicos como mentales, es crucial implementar programas de prevención de lesiones y un acompañamiento psicológico más cercano.
+El sistema de gestión propuesto debe incorporar estas áreas de mejora para optimizar el rendimiento deportivo y reducir las tasas de deserción, garantizando que los atletas se sientan apoyados tanto en el ámbito deportivo como en el personal.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1250,6 +1361,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1772,7 +1890,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1825,6 +1943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1852,6 +1971,15 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1870,6 +1998,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1891,6 +2025,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1903,9 +2064,6 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1927,6 +2085,30 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2017,6 +2199,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2087,31 +2278,31 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2143,97 +2334,33 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2885,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:K52"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2904,18 +3031,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
+      <c r="A1" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
       <c r="K1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2926,16 +3053,16 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="97"/>
       <c r="K2" s="10" t="s">
         <v>7</v>
       </c>
@@ -2946,745 +3073,745 @@
       <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:17" ht="52.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:17" ht="57.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:17" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:17" ht="132" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="36"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="81"/>
+      <c r="A8" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="102"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="102"/>
+      <c r="H8" s="102"/>
+      <c r="I8" s="102"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="103"/>
     </row>
     <row r="9" spans="1:17" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="82" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84"/>
+      <c r="A9" s="104" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
+      <c r="E9" s="105"/>
+      <c r="F9" s="105"/>
+      <c r="G9" s="105"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="106"/>
     </row>
     <row r="10" spans="1:17" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
+      <c r="A10" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="1:17" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
+      <c r="A12" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="84"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="106"/>
     </row>
     <row r="14" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="77"/>
+        <v>30</v>
+      </c>
+      <c r="B14" s="100" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="99"/>
     </row>
     <row r="15" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="99"/>
+    </row>
+    <row r="16" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="98"/>
+      <c r="C16" s="98"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="98"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="98"/>
+      <c r="K16" s="99"/>
+    </row>
+    <row r="17" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="77"/>
-    </row>
-    <row r="16" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="93"/>
+    </row>
+    <row r="18" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="46"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="77"/>
-    </row>
-    <row r="17" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="69" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="71"/>
-    </row>
-    <row r="18" spans="1:14" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="85" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="55" t="s">
+      <c r="D19" s="70"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="46" t="s">
+      <c r="H19" s="76"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="143"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="K19" s="143"/>
+      <c r="K19" s="76"/>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="145"/>
-      <c r="H20" s="146"/>
-      <c r="I20" s="147"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="146"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="79"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="145"/>
-      <c r="H21" s="146"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="145"/>
-      <c r="K21" s="146"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="79"/>
     </row>
     <row r="22" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="148"/>
-      <c r="H22" s="149"/>
-      <c r="I22" s="150"/>
-      <c r="J22" s="148"/>
-      <c r="K22" s="149"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="81"/>
+      <c r="K22" s="82"/>
     </row>
     <row r="23" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="160" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="161"/>
-      <c r="D23" s="161"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="161"/>
-      <c r="K23" s="162"/>
+        <v>56</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="163"/>
+        <v>55</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="48"/>
     </row>
     <row r="25" spans="1:14" ht="46.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="163"/>
+        <v>58</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="48"/>
     </row>
     <row r="26" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="151" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="152"/>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152"/>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="152"/>
-      <c r="J26" s="152"/>
-      <c r="K26" s="153"/>
+      <c r="B26" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="58"/>
     </row>
     <row r="27" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="154"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="155"/>
-      <c r="E27" s="155"/>
-      <c r="F27" s="155"/>
-      <c r="G27" s="155"/>
-      <c r="H27" s="155"/>
-      <c r="I27" s="155"/>
-      <c r="J27" s="155"/>
-      <c r="K27" s="156"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="61"/>
     </row>
     <row r="28" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="157"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="158"/>
-      <c r="F28" s="158"/>
-      <c r="G28" s="158"/>
-      <c r="H28" s="158"/>
-      <c r="I28" s="158"/>
-      <c r="J28" s="158"/>
-      <c r="K28" s="159"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="64"/>
     </row>
     <row r="29" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="52"/>
+      <c r="A29" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="67"/>
     </row>
     <row r="30" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="52"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="67"/>
     </row>
     <row r="31" spans="1:14" ht="28.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="52"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
+      <c r="K31" s="67"/>
     </row>
     <row r="32" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="50"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="52"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="67"/>
     </row>
     <row r="33" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="52"/>
+        <v>33</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="67"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="45"/>
+      <c r="A34" s="86" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="51"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="64"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="45"/>
+      <c r="A35" s="86"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="51"/>
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="64"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="45"/>
+      <c r="A36" s="86"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="51"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="64"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="45"/>
+      <c r="A37" s="86"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="51"/>
     </row>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="64"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="45"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="51"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="64"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="45"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="51"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="62"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
-      <c r="H40" s="62"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="63"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="84"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="84"/>
+      <c r="I40" s="84"/>
+      <c r="J40" s="84"/>
+      <c r="K40" s="85"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-      <c r="H41" s="62"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="62"/>
-      <c r="K41" s="63"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="84" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="85"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="62" t="s">
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="84"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="84"/>
+      <c r="I42" s="84"/>
+      <c r="J42" s="84"/>
+      <c r="K42" s="85"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="51"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="51"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="49"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="51"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="51"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="62"/>
-      <c r="K42" s="63"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="45"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="43"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="45"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="43"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="45"/>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="43"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="45"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="45"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="51"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="45"/>
+      <c r="A48" s="49"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="K48" s="51"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="43"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="45"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="51"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="43"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="45"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="51"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="44"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="45"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="51"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
-      <c r="B52" s="67"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
-      <c r="K52" s="68"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="89"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="89"/>
+      <c r="H52" s="89"/>
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="37">
@@ -3750,26 +3877,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="113"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="88"/>
+      <c r="A2" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -3795,60 +3922,60 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="164">
+      <c r="A4" s="28">
         <v>45597</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
+        <v>45601</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="164">
-        <v>45601</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="164">
+      <c r="A6" s="28">
         <v>45606</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3926,10 +4053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E9"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3939,241 +4066,422 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="103"/>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
+      <c r="A2" s="128"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="103"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
+      <c r="A3" s="128"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="104"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
+      <c r="A4" s="129"/>
+      <c r="B4" s="129"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
     </row>
     <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="119"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
+        <v>36</v>
+      </c>
+      <c r="B6" s="120" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
+        <v>39</v>
+      </c>
+      <c r="B7" s="84" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
+      <c r="A8" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="98"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="123"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
-      <c r="B11" s="100"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="101"/>
+      <c r="A11" s="124"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
+      <c r="A12" s="124"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="102"/>
+        <v>37</v>
+      </c>
+      <c r="B13" s="120" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="120"/>
+      <c r="D13" s="120"/>
+      <c r="E13" s="127"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="102"/>
+      <c r="B14" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="95"/>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="102"/>
+      <c r="B15" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="105" t="s">
+      <c r="A16" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
+      <c r="B16" s="130"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="95"/>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95"/>
+      <c r="A17" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="120"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
+      <c r="A18" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="62"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
+      <c r="A19" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="84"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
+      <c r="A20" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
+      <c r="A21" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
+      <c r="A22" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
+      <c r="A23" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="62"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
+      <c r="A24" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="62"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
+      <c r="A25" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="62"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
+      <c r="A27" s="84" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
+      <c r="A28" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
+      <c r="A29" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
+      <c r="A30" s="84" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="84"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="116"/>
+      <c r="C31" s="116"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="114" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="115" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="114" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
+      <c r="E36" s="114"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="50"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="114" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" s="114"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="114"/>
+      <c r="E38" s="114"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="84"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="114"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="114"/>
+      <c r="E40" s="114"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="84"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="114"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="114"/>
+      <c r="D42" s="114"/>
+      <c r="E42" s="114"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="84"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="114"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="114"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="84"/>
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="114"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="114"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="114"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="84"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="114"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="114"/>
+      <c r="D48" s="114"/>
+      <c r="E48" s="114"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="84"/>
+      <c r="B49" s="84"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="44">
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A30:E30"/>
@@ -4199,6 +4507,25 @@
     <mergeCell ref="A10:E12"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4220,157 +4547,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="149" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
     </row>
     <row r="2" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="133"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="136"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
-      <c r="B4" s="113"/>
-      <c r="C4" s="113"/>
-      <c r="D4" s="113"/>
-      <c r="E4" s="114"/>
+      <c r="A4" s="137"/>
+      <c r="B4" s="138"/>
+      <c r="C4" s="138"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="139"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="115"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="117"/>
+      <c r="A5" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="142"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="118"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="120"/>
+      <c r="A6" s="143"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="145"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="118"/>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="120"/>
+      <c r="A7" s="143"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="145"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="118"/>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="120"/>
+      <c r="A8" s="143"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="144"/>
+      <c r="E8" s="145"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="118"/>
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="120"/>
+      <c r="A9" s="143"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144"/>
+      <c r="E9" s="145"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="118"/>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="120"/>
+      <c r="A10" s="143"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="144"/>
+      <c r="E10" s="145"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="118"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="120"/>
+      <c r="A11" s="143"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="145"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="118"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="119"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="120"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="145"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="118"/>
-      <c r="B13" s="119"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="120"/>
+      <c r="A13" s="143"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="145"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="118"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="120"/>
+      <c r="A14" s="143"/>
+      <c r="B14" s="144"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="145"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="118"/>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="120"/>
+      <c r="A15" s="143"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="118"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="120"/>
+      <c r="A16" s="143"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="145"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="120"/>
+      <c r="A17" s="143"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="120"/>
+      <c r="A18" s="143"/>
+      <c r="B18" s="144"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="145"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
-      <c r="B19" s="119"/>
-      <c r="C19" s="119"/>
-      <c r="D19" s="119"/>
-      <c r="E19" s="120"/>
+      <c r="A19" s="143"/>
+      <c r="B19" s="144"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="144"/>
+      <c r="E19" s="145"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="118"/>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="120"/>
+      <c r="A20" s="143"/>
+      <c r="B20" s="144"/>
+      <c r="C20" s="144"/>
+      <c r="D20" s="144"/>
+      <c r="E20" s="145"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="121"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122"/>
-      <c r="E21" s="123"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="147"/>
+      <c r="C21" s="147"/>
+      <c r="D21" s="147"/>
+      <c r="E21" s="148"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4388,218 +4717,218 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="98.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="127"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="152"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="153" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="130"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="155"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="131"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="133"/>
+      <c r="A3" s="156"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="158"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="136"/>
+      <c r="A4" s="159" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="161"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="137"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="139"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="137"/>
-      <c r="B6" s="138"/>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="139"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="137"/>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="139"/>
+      <c r="A7" s="162"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="139"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="138"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="139"/>
+      <c r="A9" s="162"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="137"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
+      <c r="A10" s="162"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="164"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="139"/>
+      <c r="A11" s="162"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="163"/>
+      <c r="G11" s="164"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="139"/>
+      <c r="A12" s="162"/>
+      <c r="B12" s="163"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="164"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="137"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="139"/>
+      <c r="A13" s="162"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="164"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="139"/>
+      <c r="A14" s="162"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="164"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="139"/>
+      <c r="A15" s="162"/>
+      <c r="B15" s="163"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="164"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="139"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="164"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="137"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="139"/>
+      <c r="A17" s="162"/>
+      <c r="B17" s="163"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="164"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="139"/>
+      <c r="A18" s="162"/>
+      <c r="B18" s="163"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="164"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="139"/>
+      <c r="A19" s="162"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="164"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="139"/>
+      <c r="A20" s="162"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="163"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="164"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="137"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="139"/>
+      <c r="A21" s="162"/>
+      <c r="B21" s="163"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="164"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="140"/>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="142"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="166"/>
+      <c r="D22" s="166"/>
+      <c r="E22" s="166"/>
+      <c r="F22" s="166"/>
+      <c r="G22" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4616,8 +4945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4626,208 +4955,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="150" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="127"/>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="152"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="153" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="130"/>
+      <c r="B2" s="154"/>
+      <c r="C2" s="154"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="155"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="131"/>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="133"/>
+      <c r="A3" s="156"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="158"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="134" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="135"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="136"/>
+      <c r="A4" s="159" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="161"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="137"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="139"/>
+      <c r="A5" s="162"/>
+      <c r="B5" s="163"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="137"/>
-      <c r="B6" s="138"/>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="139"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="163"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="137"/>
-      <c r="B7" s="138"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="139"/>
+      <c r="A7" s="162"/>
+      <c r="B7" s="163"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="137"/>
-      <c r="B8" s="138"/>
-      <c r="C8" s="138"/>
-      <c r="D8" s="138"/>
-      <c r="E8" s="138"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="139"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
-      <c r="B9" s="138"/>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="139"/>
+      <c r="A9" s="162"/>
+      <c r="B9" s="163"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="137"/>
-      <c r="B10" s="138"/>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="138"/>
-      <c r="F10" s="138"/>
-      <c r="G10" s="139"/>
+      <c r="A10" s="162"/>
+      <c r="B10" s="163"/>
+      <c r="C10" s="163"/>
+      <c r="D10" s="163"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="163"/>
+      <c r="G10" s="164"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="137"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="139"/>
+      <c r="A11" s="162"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="163"/>
+      <c r="G11" s="164"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="137"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="139"/>
+      <c r="A12" s="162"/>
+      <c r="B12" s="163"/>
+      <c r="C12" s="163"/>
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
+      <c r="F12" s="163"/>
+      <c r="G12" s="164"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="137"/>
-      <c r="B13" s="138"/>
-      <c r="C13" s="138"/>
-      <c r="D13" s="138"/>
-      <c r="E13" s="138"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="139"/>
+      <c r="A13" s="162"/>
+      <c r="B13" s="163"/>
+      <c r="C13" s="163"/>
+      <c r="D13" s="163"/>
+      <c r="E13" s="163"/>
+      <c r="F13" s="163"/>
+      <c r="G13" s="164"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="137"/>
-      <c r="B14" s="138"/>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="138"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="139"/>
+      <c r="A14" s="162"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="163"/>
+      <c r="D14" s="163"/>
+      <c r="E14" s="163"/>
+      <c r="F14" s="163"/>
+      <c r="G14" s="164"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="137"/>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="139"/>
+      <c r="A15" s="162"/>
+      <c r="B15" s="163"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="163"/>
+      <c r="E15" s="163"/>
+      <c r="F15" s="163"/>
+      <c r="G15" s="164"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="137"/>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="139"/>
+      <c r="A16" s="162"/>
+      <c r="B16" s="163"/>
+      <c r="C16" s="163"/>
+      <c r="D16" s="163"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="163"/>
+      <c r="G16" s="164"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="137"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="139"/>
+      <c r="A17" s="162"/>
+      <c r="B17" s="163"/>
+      <c r="C17" s="163"/>
+      <c r="D17" s="163"/>
+      <c r="E17" s="163"/>
+      <c r="F17" s="163"/>
+      <c r="G17" s="164"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="137"/>
-      <c r="B18" s="138"/>
-      <c r="C18" s="138"/>
-      <c r="D18" s="138"/>
-      <c r="E18" s="138"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="139"/>
+      <c r="A18" s="162"/>
+      <c r="B18" s="163"/>
+      <c r="C18" s="163"/>
+      <c r="D18" s="163"/>
+      <c r="E18" s="163"/>
+      <c r="F18" s="163"/>
+      <c r="G18" s="164"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="137"/>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="139"/>
+      <c r="A19" s="162"/>
+      <c r="B19" s="163"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="163"/>
+      <c r="E19" s="163"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="164"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="137"/>
-      <c r="B20" s="138"/>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="138"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="139"/>
+      <c r="A20" s="162"/>
+      <c r="B20" s="163"/>
+      <c r="C20" s="163"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="163"/>
+      <c r="F20" s="163"/>
+      <c r="G20" s="164"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="137"/>
-      <c r="B21" s="138"/>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="139"/>
+      <c r="A21" s="162"/>
+      <c r="B21" s="163"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
+      <c r="F21" s="163"/>
+      <c r="G21" s="164"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="140"/>
-      <c r="B22" s="141"/>
-      <c r="C22" s="141"/>
-      <c r="D22" s="141"/>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="142"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="166"/>
+      <c r="D22" s="166"/>
+      <c r="E22" s="166"/>
+      <c r="F22" s="166"/>
+      <c r="G22" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>